<commit_message>
added updates to python flask layout
</commit_message>
<xml_diff>
--- a/B2B Data Provider-sample1.xlsx
+++ b/B2B Data Provider-sample1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Everything On This PC\Udacity\Git_hseju\SoftwareRecommender\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29682AF0-5DE9-4959-BFAF-05A51BD697D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD937741-F8C9-4CBA-A108-63C7BDD27C6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -623,7 +623,7 @@
     <col min="6" max="8" width="20.1328125" customWidth="1"/>
     <col min="9" max="9" width="23.06640625" customWidth="1"/>
     <col min="11" max="11" width="70.53125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="40.1328125" customWidth="1"/>
+    <col min="12" max="12" width="39.59765625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="29.19921875" customWidth="1"/>
     <col min="14" max="14" width="17.53125" customWidth="1"/>
     <col min="15" max="15" width="21.3984375" customWidth="1"/>

</xml_diff>

<commit_message>
update on email function
</commit_message>
<xml_diff>
--- a/B2B Data Provider-sample1.xlsx
+++ b/B2B Data Provider-sample1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Everything On This PC\Udacity\Git_hseju\SoftwareRecommender\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D25C6FF-E4BE-4CDA-A32F-0CA0A4F12BD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5935BF-D9A9-45A1-B4CB-B6A5045FE05F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="113">
   <si>
     <t>Company</t>
   </si>
@@ -351,6 +351,18 @@
   <si>
     <t>396,</t>
   </si>
+  <si>
+    <t>credits</t>
+  </si>
+  <si>
+    <t>5, 2040, 4800, 12000</t>
+  </si>
+  <si>
+    <t>1000,5000, 20000, 50000, 100000</t>
+  </si>
+  <si>
+    <t>10, 250, 1000</t>
+  </si>
 </sst>
 </file>
 
@@ -432,7 +444,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -455,6 +467,7 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -673,13 +686,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:T999"/>
+  <dimension ref="A1:U999"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="S2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomRight" activeCell="V8" sqref="V8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -696,9 +709,11 @@
     <col min="16" max="16" width="17.53125" customWidth="1"/>
     <col min="17" max="17" width="21.3984375" customWidth="1"/>
     <col min="19" max="19" width="70.59765625" customWidth="1"/>
+    <col min="20" max="20" width="16.06640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="28.9296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="46.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" ht="46.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -759,8 +774,11 @@
       <c r="T1" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" ht="89.25" x14ac:dyDescent="0.35">
+      <c r="U1" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="89.25" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -818,8 +836,11 @@
       <c r="T2" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="U2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -880,8 +901,11 @@
       <c r="T3" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="U3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
@@ -936,8 +960,11 @@
       <c r="T4" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" ht="78" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="U4" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="78" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>29</v>
       </c>
@@ -993,7 +1020,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="25.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:21" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>33</v>
       </c>
@@ -1054,8 +1081,11 @@
       <c r="T6" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="U6" s="10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>40</v>
       </c>
@@ -1111,7 +1141,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="37.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" ht="37.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>44</v>
       </c>
@@ -1170,7 +1200,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="31.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:21" ht="31.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>48</v>
       </c>
@@ -1232,7 +1262,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="36.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" ht="36.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>54</v>
       </c>
@@ -1289,7 +1319,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
         <v>59</v>
       </c>
@@ -1344,8 +1374,11 @@
       <c r="T11" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="U11" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -1356,7 +1389,7 @@
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
     </row>
-    <row r="13" spans="1:20" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -1367,7 +1400,7 @@
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
     </row>
-    <row r="14" spans="1:20" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -1378,7 +1411,7 @@
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
     </row>
-    <row r="15" spans="1:20" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -1389,7 +1422,7 @@
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
     </row>
-    <row r="16" spans="1:20" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:21" ht="12.75" x14ac:dyDescent="0.35">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>

</xml_diff>

<commit_message>
Added updated data file
</commit_message>
<xml_diff>
--- a/B2B Data Provider-sample1.xlsx
+++ b/B2B Data Provider-sample1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Everything On This PC\Udacity\Git_hseju\SoftwareRecommender\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5251915B-F215-4243-9ADA-817ABBB7A54D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42ECF10E-6521-4423-9381-094C58F03F6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="147">
   <si>
     <t>Company</t>
   </si>
@@ -302,9 +302,6 @@
   </si>
   <si>
     <t>0, 147</t>
-  </si>
-  <si>
-    <t>29, 49</t>
   </si>
   <si>
     <t>39, 99, 189,369,738</t>
@@ -855,10 +852,10 @@
   <dimension ref="A1:AQ999"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomRight" activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -944,73 +941,73 @@
         <v>71</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="V1" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="W1" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="W1" s="14" t="s">
+      <c r="X1" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="X1" s="14" t="s">
+      <c r="Y1" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="Y1" s="14" t="s">
+      <c r="Z1" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="Z1" s="14" t="s">
+      <c r="AA1" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="AA1" s="14" t="s">
+      <c r="AB1" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="AB1" s="14" t="s">
+      <c r="AC1" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="AC1" s="14" t="s">
+      <c r="AD1" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="AD1" s="14" t="s">
+      <c r="AE1" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="AE1" s="14" t="s">
+      <c r="AF1" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="AF1" s="14" t="s">
+      <c r="AG1" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="AG1" s="14" t="s">
+      <c r="AH1" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="AH1" s="14" t="s">
+      <c r="AI1" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="AI1" s="14" t="s">
+      <c r="AJ1" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="AJ1" s="14" t="s">
+      <c r="AK1" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="AK1" s="14" t="s">
+      <c r="AL1" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="AL1" s="14" t="s">
+      <c r="AM1" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="AM1" s="14" t="s">
+      <c r="AN1" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="AN1" s="14" t="s">
+      <c r="AO1" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="AO1" s="14" t="s">
+      <c r="AP1" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="AP1" s="11" t="s">
-        <v>120</v>
-      </c>
       <c r="AQ1" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:43" ht="89.25" x14ac:dyDescent="0.35">
@@ -1018,10 +1015,10 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D2" s="9">
         <v>11995</v>
@@ -1096,7 +1093,7 @@
         <v>34995</v>
       </c>
       <c r="AC2" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AD2" s="14" t="s">
         <v>14</v>
@@ -1136,7 +1133,7 @@
       </c>
       <c r="AP2" s="11"/>
       <c r="AQ2" s="19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:43" ht="25.5" x14ac:dyDescent="0.35">
@@ -1144,10 +1141,10 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D3" s="9">
         <v>16500</v>
@@ -1198,7 +1195,7 @@
         <v>24</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="U3" s="1" t="s">
         <v>14</v>
@@ -1207,7 +1204,7 @@
         <v>16500</v>
       </c>
       <c r="W3" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="X3" s="14" t="s">
         <v>14</v>
@@ -1265,7 +1262,7 @@
       </c>
       <c r="AP3" s="11"/>
       <c r="AQ3" s="19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:43" ht="25.5" x14ac:dyDescent="0.35">
@@ -1273,7 +1270,7 @@
         <v>25</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>91</v>
@@ -1324,7 +1321,7 @@
         <v>82</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="V4" s="16">
         <v>890</v>
@@ -1348,7 +1345,7 @@
         <v>14</v>
       </c>
       <c r="AC4" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AD4" s="14" t="s">
         <v>14</v>
@@ -1388,7 +1385,7 @@
       </c>
       <c r="AP4" s="11"/>
       <c r="AQ4" s="19" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="78" customHeight="1" x14ac:dyDescent="0.35">
@@ -1462,7 +1459,7 @@
         <v>14</v>
       </c>
       <c r="AA5" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AB5" s="14" t="s">
         <v>14</v>
@@ -1516,10 +1513,10 @@
         <v>33</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D6" s="9">
         <v>0</v>
@@ -1573,25 +1570,25 @@
         <v>82</v>
       </c>
       <c r="U6" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="V6" s="16">
         <v>468</v>
       </c>
       <c r="W6" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="X6" s="16">
         <v>948</v>
       </c>
       <c r="Y6" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Z6" s="16">
         <v>6000</v>
       </c>
       <c r="AA6" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AB6" s="14" t="s">
         <v>14</v>
@@ -1609,13 +1606,13 @@
         <v>49</v>
       </c>
       <c r="AG6" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AH6" s="16">
         <v>99</v>
       </c>
       <c r="AI6" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AJ6" s="14" t="s">
         <v>14</v>
@@ -1636,10 +1633,10 @@
         <v>14</v>
       </c>
       <c r="AP6" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AQ6" s="19" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:43" ht="25.5" x14ac:dyDescent="0.35">
@@ -1650,7 +1647,7 @@
         <v>92</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D7" s="9">
         <v>1764</v>
@@ -1713,7 +1710,7 @@
         <v>9528</v>
       </c>
       <c r="AA7" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AB7" s="14" t="s">
         <v>14</v>
@@ -1759,7 +1756,7 @@
       </c>
       <c r="AP7" s="11"/>
       <c r="AQ7" s="20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:43" ht="37.9" customHeight="1" x14ac:dyDescent="0.35">
@@ -1767,10 +1764,10 @@
         <v>44</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D8" s="9">
         <v>468</v>
@@ -1881,7 +1878,7 @@
         <v>14</v>
       </c>
       <c r="AP8" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AQ8" s="20" t="s">
         <v>47</v>
@@ -1892,10 +1889,10 @@
         <v>48</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D9" s="9">
         <v>348</v>
@@ -2009,7 +2006,7 @@
         <v>14</v>
       </c>
       <c r="AP9" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AQ9" s="20" t="s">
         <v>51</v>
@@ -2020,10 +2017,10 @@
         <v>54</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D10" s="9">
         <v>0</v>
@@ -2042,7 +2039,7 @@
         <v>55</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>69</v>
+        <v>15</v>
       </c>
       <c r="K10" s="5" t="s">
         <v>56</v>
@@ -2063,7 +2060,7 @@
         <v>38</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="S10" s="1" t="s">
         <v>58</v>
@@ -2075,7 +2072,7 @@
         <v>2000</v>
       </c>
       <c r="W10" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="X10" s="14" t="s">
         <v>14</v>
@@ -2132,10 +2129,10 @@
         <v>14</v>
       </c>
       <c r="AP10" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AQ10" s="20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:43" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2143,10 +2140,10 @@
         <v>59</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D11" s="9">
         <v>39</v>
@@ -2164,7 +2161,7 @@
         <v>61</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>15</v>
+        <v>69</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>56</v>
@@ -2194,7 +2191,7 @@
         <v>82</v>
       </c>
       <c r="U11" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="V11" s="16">
         <v>396</v>
@@ -2224,7 +2221,7 @@
         <v>7380</v>
       </c>
       <c r="AE11" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AF11" s="16">
         <v>39</v>
@@ -2254,13 +2251,13 @@
         <v>738</v>
       </c>
       <c r="AO11" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AP11" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AQ11" s="19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:43" ht="12.75" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
added changes to rec.py
</commit_message>
<xml_diff>
--- a/B2B Data Provider-sample1.xlsx
+++ b/B2B Data Provider-sample1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Everything On This PC\Udacity\Git_hseju\SoftwareRecommender\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D44C4E27-C010-4301-92EB-84DA4455A3B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4281208-FB21-4DE3-A2DE-D3ACF287B878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -462,13 +462,13 @@
     <t>468, 948, 6000</t>
   </si>
   <si>
+    <t>16500, 27500</t>
+  </si>
+  <si>
+    <t>348, 588, 2000</t>
+  </si>
+  <si>
     <t>USA/NorthAmerica,International</t>
-  </si>
-  <si>
-    <t>16500, 27500</t>
-  </si>
-  <si>
-    <t>348, 588, 2000</t>
   </si>
 </sst>
 </file>
@@ -852,10 +852,10 @@
   <dimension ref="A1:AQ999"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomRight" activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -872,7 +872,7 @@
     <col min="16" max="16" width="17.53125" customWidth="1"/>
     <col min="17" max="17" width="21.3984375" customWidth="1"/>
     <col min="19" max="19" width="70.59765625" customWidth="1"/>
-    <col min="20" max="20" width="26.265625" customWidth="1"/>
+    <col min="20" max="20" width="35.06640625" customWidth="1"/>
     <col min="21" max="21" width="28.9296875" bestFit="1" customWidth="1"/>
     <col min="22" max="41" width="12.59765625" style="17"/>
     <col min="42" max="42" width="88.3984375" bestFit="1" customWidth="1"/>
@@ -1144,7 +1144,7 @@
         <v>94</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D3" s="9">
         <v>16500</v>
@@ -1195,7 +1195,7 @@
         <v>24</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="U3" s="1" t="s">
         <v>14</v>
@@ -2020,7 +2020,7 @@
         <v>94</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D10" s="9">
         <v>0</v>

</xml_diff>